<commit_message>
predeployment sprint 2. Cybersource veitin, Cybersource paymaya, 7Eleven, Cybersource OCBC, Cybersource OCBC MDR
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Dispatcher_Portal/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Dispatcher_Portal/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\Kalyana\Traveloka_DataAutomation_Dispatcher_Portal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DD5B33-1B08-4858-9814-6F6F95A05DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B183CE-F8DE-45F8-B728-F807F22696AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3552" yWindow="1236" windowWidth="17280" windowHeight="9000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -181,28 +181,28 @@
     <t>PathSAKey</t>
   </si>
   <si>
+    <t>RPA_Moon_Cred_Gmail</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMasterFolder</t>
+  </si>
+  <si>
+    <t>RPA_Moon_SheetIdConfig</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
     <t>EmailSenderName</t>
   </si>
   <si>
     <t>RPA_Moon_SenderName</t>
   </si>
   <si>
-    <t>[DEV] RPA_Moon_SheetIdConfig</t>
-  </si>
-  <si>
-    <t>[DEV] RPA_Moon_PathMasterFolder</t>
-  </si>
-  <si>
-    <t>[DEV] RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
-    <t>[DEV] RPA_Moon_PathSaKey</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_Portal</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_Cred_Gmail</t>
+    <t>RPA_Moon_Portal</t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -633,7 +633,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -671,7 +671,7 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
@@ -2838,8 +2838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -2899,7 +2899,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
@@ -2907,7 +2907,7 @@
         <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.3" customHeight="1">
@@ -2915,15 +2915,15 @@
         <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1"/>

</xml_diff>

<commit_message>
Update Pre SIT Molpay SGD & SGD Fee
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Dispatcher_Portal/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Dispatcher_Portal/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\Kalyana\Traveloka_DataAutomation_Dispatcher_Portal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B183CE-F8DE-45F8-B728-F807F22696AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DD5B33-1B08-4858-9814-6F6F95A05DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3552" yWindow="1236" windowWidth="17280" windowHeight="9000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -181,28 +181,28 @@
     <t>PathSAKey</t>
   </si>
   <si>
-    <t>RPA_Moon_Cred_Gmail</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathMasterFolder</t>
-  </si>
-  <si>
-    <t>RPA_Moon_SheetIdConfig</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathSaKey</t>
-  </si>
-  <si>
     <t>EmailSenderName</t>
   </si>
   <si>
     <t>RPA_Moon_SenderName</t>
   </si>
   <si>
-    <t>RPA_Moon_Portal</t>
+    <t>[DEV] RPA_Moon_SheetIdConfig</t>
+  </si>
+  <si>
+    <t>[DEV] RPA_Moon_PathMasterFolder</t>
+  </si>
+  <si>
+    <t>[DEV] RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>[DEV] RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_Portal</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_Cred_Gmail</t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -633,7 +633,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -671,7 +671,7 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
@@ -2838,8 +2838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -2899,7 +2899,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
@@ -2907,7 +2907,7 @@
         <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.3" customHeight="1">
@@ -2915,15 +2915,15 @@
         <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1"/>

</xml_diff>

<commit_message>
Update Dispatcher param ProductType
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Dispatcher_Portal/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Dispatcher_Portal/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Dispatcher_Portal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192C459B-F33E-43F3-9802-CCC999DEE184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D7CED9-92DA-4997-92EC-8BE83FFB7FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="984" yWindow="12852" windowWidth="22320" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -205,9 +205,6 @@
     <t>[Dev] RPA_Moon_Cred_Gmail</t>
   </si>
   <si>
-    <t>SheetIdConfigAccomodation</t>
-  </si>
-  <si>
     <t>[Dev] RPA_Moon_SheetIdConfig_Accommodation</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>[Dev] RPA_Moon_SheetIdConfig_Transport</t>
+  </si>
+  <si>
+    <t>SheetIdConfigAccommodation</t>
   </si>
 </sst>
 </file>
@@ -598,12 +598,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" customWidth="1"/>
+    <col min="1" max="1" width="43.44140625" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -651,7 +651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -661,7 +661,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1694,12 +1694,12 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1736,7 +1736,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1861,7 +1861,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2857,15 +2857,15 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="60.44140625" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2946,18 +2946,18 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
         <v>59</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
         <v>61</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Update sheet BMG & RWS, Fix typo malindo
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Dispatcher_Portal/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Dispatcher_Portal/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Dispatcher_Portal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D7CED9-92DA-4997-92EC-8BE83FFB7FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4655ACEE-E2E4-410B-8E4E-BCFB51642622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -215,6 +215,18 @@
   </si>
   <si>
     <t>SheetIdConfigAccommodation</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_SheetIdConfig_InterCon</t>
+  </si>
+  <si>
+    <t>SheetIdConfigIntercon</t>
+  </si>
+  <si>
+    <t>SheetIdConfigExperience</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_SheetIdConfig_Experience</t>
   </si>
 </sst>
 </file>
@@ -296,9 +308,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -336,7 +348,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -442,7 +454,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -584,7 +596,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -594,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2856,8 +2868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2960,8 +2972,22 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Update resortworldsentosa wait element navigate to download report
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Dispatcher_Portal/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Dispatcher_Portal/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Dispatcher_Portal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A329ED7B-6552-48F9-B0BB-78E4057E84D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0E2E20-7CF3-4C16-B725-E075EBA14CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23232" windowHeight="11496" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,46 +187,46 @@
     <t>RPA_Moon_SenderName</t>
   </si>
   <si>
+    <t>[DEV] RPA_Moon_SheetIdConfig</t>
+  </si>
+  <si>
+    <t>[DEV] RPA_Moon_PathMasterFolder</t>
+  </si>
+  <si>
+    <t>[DEV] RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>[DEV] RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_Portal</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_Cred_Gmail</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_SheetIdConfig_Accommodation</t>
+  </si>
+  <si>
     <t>SheetIdConfigTransport</t>
   </si>
   <si>
+    <t>[Dev] RPA_Moon_SheetIdConfig_Transport</t>
+  </si>
+  <si>
     <t>SheetIdConfigAccommodation</t>
   </si>
   <si>
     <t>SheetIdConfigExperience</t>
   </si>
   <si>
-    <t>RPA_Moon_Portal</t>
-  </si>
-  <si>
-    <t>RPA_Moon_Cred_Gmail</t>
-  </si>
-  <si>
-    <t>RPA_Moon_SheetIdConfig</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathMasterFolder</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathSaKey</t>
-  </si>
-  <si>
-    <t>RPA_Moon_SheetIdConfig_Accommodation</t>
-  </si>
-  <si>
-    <t>RPA_Moon_SheetIdConfig_Transport</t>
-  </si>
-  <si>
-    <t>RPA_Moon_SheetIdConfig_Experience</t>
+    <t>[Dev] RPA_Moon_SheetIdConfig_Experience</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_SheetIdConfig_IC</t>
   </si>
   <si>
     <t>SheetIdConfigIC</t>
-  </si>
-  <si>
-    <t>RPA_Moon_SheetIdConfig_IC</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="14.95" customHeight="1"/>
@@ -657,7 +657,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -695,7 +695,7 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
@@ -2869,7 +2869,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="14.95" customHeight="1"/>
@@ -2921,7 +2921,7 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.3" customHeight="1">
@@ -2929,7 +2929,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
@@ -2937,7 +2937,7 @@
         <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.3" customHeight="1">
@@ -2945,7 +2945,7 @@
         <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
@@ -2958,31 +2958,31 @@
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1">
       <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
         <v>65</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.3" customHeight="1">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
         <v>64</v>

</xml_diff>